<commit_message>
Final Changes to PCB, more code for gateway
</commit_message>
<xml_diff>
--- a/Power Budget.xlsx
+++ b/Power Budget.xlsx
@@ -1,16 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="26626"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="26731"/>
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="https://uctcloud-my.sharepoint.com/personal/rssmik001_myuct_ac_za/Documents/EEE4022S Report/LAS-Laboratory-Access-System/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="18" documentId="8_{066A72DA-FEC3-4DAC-93CC-A281EBAD5DCB}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{AEA5A423-DBC8-4321-ACDC-849B4043A757}"/>
+  <xr:revisionPtr revIDLastSave="56" documentId="8_{066A72DA-FEC3-4DAC-93CC-A281EBAD5DCB}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{D4E31DCF-06AA-46AA-A48C-D8F27B37C0FE}"/>
   <bookViews>
-    <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="16440" xr2:uid="{0249F443-B095-48D9-A27F-C54B977A2593}"/>
+    <workbookView xWindow="-98" yWindow="-98" windowWidth="24196" windowHeight="13695" xr2:uid="{0249F443-B095-48D9-A27F-C54B977A2593}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -47,16 +47,16 @@
     <t>CH343C</t>
   </si>
   <si>
-    <t>Relay(USES 5V)</t>
-  </si>
-  <si>
-    <t>Active mode</t>
-  </si>
-  <si>
-    <t>and TX</t>
-  </si>
-  <si>
-    <t>and RX</t>
+    <t>Maximum Current Draw (mA)</t>
+  </si>
+  <si>
+    <t>LEDs</t>
+  </si>
+  <si>
+    <t>WS2812B</t>
+  </si>
+  <si>
+    <t>Total</t>
   </si>
 </sst>
 </file>
@@ -80,15 +80,21 @@
       <scheme val="minor"/>
     </font>
   </fonts>
-  <fills count="2">
+  <fills count="3">
     <fill>
       <patternFill patternType="none"/>
     </fill>
     <fill>
       <patternFill patternType="gray125"/>
     </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="0"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
   </fills>
-  <borders count="1">
+  <borders count="3">
     <border>
       <left/>
       <right/>
@@ -96,13 +102,48 @@
       <bottom/>
       <diagonal/>
     </border>
+    <border>
+      <left style="thin">
+        <color indexed="64"/>
+      </left>
+      <right style="thin">
+        <color indexed="64"/>
+      </right>
+      <top style="thin">
+        <color indexed="64"/>
+      </top>
+      <bottom style="thin">
+        <color indexed="64"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left style="thin">
+        <color indexed="64"/>
+      </left>
+      <right style="thin">
+        <color indexed="64"/>
+      </right>
+      <top style="thin">
+        <color indexed="64"/>
+      </top>
+      <bottom style="double">
+        <color indexed="64"/>
+      </bottom>
+      <diagonal/>
+    </border>
   </borders>
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="2">
+  <cellXfs count="7">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="1"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="2" borderId="2" xfId="0" applyFill="1" applyBorder="1"/>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -417,65 +458,71 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{2AF74093-CB4B-4DC7-8B75-697641BAAEE8}">
-  <dimension ref="A1:B7"/>
+  <dimension ref="A1:C6"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="A3" sqref="A3:B6"/>
+      <selection activeCell="B6" sqref="A1:B6"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr defaultRowHeight="14.25" x14ac:dyDescent="0.45"/>
   <cols>
-    <col min="1" max="1" width="22.42578125" customWidth="1"/>
+    <col min="1" max="1" width="22.3984375" customWidth="1"/>
+    <col min="2" max="2" width="27.73046875" customWidth="1"/>
+    <col min="3" max="3" width="17.73046875" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A1" t="s">
+    <row r="1" spans="1:3" x14ac:dyDescent="0.45">
+      <c r="A1" s="3" t="s">
         <v>0</v>
       </c>
+      <c r="B1" s="3" t="s">
+        <v>3</v>
+      </c>
+      <c r="C1" s="1"/>
     </row>
-    <row r="2" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A2" s="1" t="s">
+    <row r="2" spans="1:3" x14ac:dyDescent="0.45">
+      <c r="A2" s="4" t="s">
         <v>1</v>
       </c>
-      <c r="B2">
-        <v>120</v>
+      <c r="B2" s="5">
+        <v>500</v>
       </c>
     </row>
-    <row r="3" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A3" t="s">
+    <row r="3" spans="1:3" x14ac:dyDescent="0.45">
+      <c r="A3" s="5" t="s">
+        <v>2</v>
+      </c>
+      <c r="B3" s="5">
+        <v>12</v>
+      </c>
+    </row>
+    <row r="4" spans="1:3" x14ac:dyDescent="0.45">
+      <c r="A4" s="5" t="s">
         <v>4</v>
       </c>
-      <c r="B3">
-        <v>24</v>
+      <c r="B4" s="5">
+        <v>6.5</v>
       </c>
     </row>
-    <row r="4" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A4" t="s">
+    <row r="5" spans="1:3" ht="14.65" thickBot="1" x14ac:dyDescent="0.5">
+      <c r="A5" s="6" t="s">
         <v>5</v>
       </c>
+      <c r="B5" s="6">
+        <v>20</v>
+      </c>
     </row>
-    <row r="5" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A5" t="s">
+    <row r="6" spans="1:3" ht="14.65" thickTop="1" x14ac:dyDescent="0.45">
+      <c r="A6" s="2" t="s">
         <v>6</v>
       </c>
-    </row>
-    <row r="6" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A6" t="s">
-        <v>2</v>
-      </c>
-      <c r="B6">
-        <v>12</v>
-      </c>
-    </row>
-    <row r="7" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A7" t="s">
-        <v>3</v>
-      </c>
-      <c r="B7">
-        <v>71</v>
+      <c r="B6" s="2">
+        <f>SUM(B2:B5)</f>
+        <v>538.5</v>
       </c>
     </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <pageSetup orientation="portrait" r:id="rId1"/>
 </worksheet>
 </file>
</xml_diff>

<commit_message>
No clue, more gateway I think
</commit_message>
<xml_diff>
--- a/Power Budget.xlsx
+++ b/Power Budget.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="https://uctcloud-my.sharepoint.com/personal/rssmik001_myuct_ac_za/Documents/EEE4022S Report/LAS-Laboratory-Access-System/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="56" documentId="8_{066A72DA-FEC3-4DAC-93CC-A281EBAD5DCB}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{D4E31DCF-06AA-46AA-A48C-D8F27B37C0FE}"/>
+  <xr:revisionPtr revIDLastSave="67" documentId="8_{066A72DA-FEC3-4DAC-93CC-A281EBAD5DCB}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{EC3034F3-ED93-4828-807C-F681D9E16648}"/>
   <bookViews>
-    <workbookView xWindow="-98" yWindow="-98" windowWidth="24196" windowHeight="13695" xr2:uid="{0249F443-B095-48D9-A27F-C54B977A2593}"/>
+    <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="16440" xr2:uid="{0249F443-B095-48D9-A27F-C54B977A2593}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -36,7 +36,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="7" uniqueCount="7">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="8" uniqueCount="8">
   <si>
     <t>Components</t>
   </si>
@@ -57,6 +57,9 @@
   </si>
   <si>
     <t>Total</t>
+  </si>
+  <si>
+    <t>Power Consumption (mW)</t>
   </si>
 </sst>
 </file>
@@ -94,7 +97,7 @@
       </patternFill>
     </fill>
   </fills>
-  <borders count="3">
+  <borders count="5">
     <border>
       <left/>
       <right/>
@@ -132,18 +135,46 @@
       </bottom>
       <diagonal/>
     </border>
+    <border>
+      <left style="thin">
+        <color indexed="64"/>
+      </left>
+      <right/>
+      <top style="thin">
+        <color indexed="64"/>
+      </top>
+      <bottom style="thin">
+        <color indexed="64"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left style="thin">
+        <color indexed="64"/>
+      </left>
+      <right/>
+      <top style="thin">
+        <color indexed="64"/>
+      </top>
+      <bottom style="double">
+        <color indexed="64"/>
+      </bottom>
+      <diagonal/>
+    </border>
   </borders>
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="7">
+  <cellXfs count="9">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1"/>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="2" borderId="2" xfId="0" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="3" xfId="0" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="2" borderId="4" xfId="0" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="2" xfId="0" applyBorder="1"/>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -461,64 +492,86 @@
   <dimension ref="A1:C6"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="B6" sqref="A1:B6"/>
+      <selection activeCell="C1" sqref="C1:C6"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="14.25" x14ac:dyDescent="0.45"/>
+  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="1" max="1" width="22.3984375" customWidth="1"/>
-    <col min="2" max="2" width="27.73046875" customWidth="1"/>
-    <col min="3" max="3" width="17.73046875" customWidth="1"/>
+    <col min="1" max="1" width="22.42578125" customWidth="1"/>
+    <col min="2" max="2" width="27.7109375" customWidth="1"/>
+    <col min="3" max="3" width="25.42578125" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:3" x14ac:dyDescent="0.45">
-      <c r="A1" s="3" t="s">
+    <row r="1" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A1" s="2" t="s">
         <v>0</v>
       </c>
-      <c r="B1" s="3" t="s">
+      <c r="B1" s="2" t="s">
         <v>3</v>
       </c>
-      <c r="C1" s="1"/>
+      <c r="C1" s="1" t="s">
+        <v>7</v>
+      </c>
     </row>
-    <row r="2" spans="1:3" x14ac:dyDescent="0.45">
-      <c r="A2" s="4" t="s">
+    <row r="2" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A2" s="3" t="s">
         <v>1</v>
       </c>
       <c r="B2" s="5">
         <v>500</v>
       </c>
+      <c r="C2" s="3">
+        <f>3.3*B2</f>
+        <v>1650</v>
+      </c>
     </row>
-    <row r="3" spans="1:3" x14ac:dyDescent="0.45">
-      <c r="A3" s="5" t="s">
+    <row r="3" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A3" s="3" t="s">
         <v>2</v>
       </c>
       <c r="B3" s="5">
         <v>12</v>
       </c>
+      <c r="C3" s="3">
+        <f t="shared" ref="C3:C6" si="0">3.3*B3</f>
+        <v>39.599999999999994</v>
+      </c>
     </row>
-    <row r="4" spans="1:3" x14ac:dyDescent="0.45">
-      <c r="A4" s="5" t="s">
+    <row r="4" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A4" s="3" t="s">
         <v>4</v>
       </c>
       <c r="B4" s="5">
         <v>6.5</v>
       </c>
+      <c r="C4" s="3">
+        <f t="shared" si="0"/>
+        <v>21.45</v>
+      </c>
     </row>
-    <row r="5" spans="1:3" ht="14.65" thickBot="1" x14ac:dyDescent="0.5">
-      <c r="A5" s="6" t="s">
+    <row r="5" spans="1:3" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="A5" s="4" t="s">
         <v>5</v>
       </c>
       <c r="B5" s="6">
         <v>20</v>
       </c>
+      <c r="C5" s="8">
+        <f t="shared" si="0"/>
+        <v>66</v>
+      </c>
     </row>
-    <row r="6" spans="1:3" ht="14.65" thickTop="1" x14ac:dyDescent="0.45">
-      <c r="A6" s="2" t="s">
+    <row r="6" spans="1:3" ht="15.75" thickTop="1" x14ac:dyDescent="0.25">
+      <c r="A6" t="s">
         <v>6</v>
       </c>
-      <c r="B6" s="2">
+      <c r="B6">
         <f>SUM(B2:B5)</f>
         <v>538.5</v>
+      </c>
+      <c r="C6" s="7">
+        <f t="shared" si="0"/>
+        <v>1777.05</v>
       </c>
     </row>
   </sheetData>

</xml_diff>